<commit_message>
No gray, juste white
</commit_message>
<xml_diff>
--- a/dataset/color_range_with_gray.xlsx
+++ b/dataset/color_range_with_gray.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projets\color_recognizer\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3ACC20-F6B3-42E4-A600-E3BD904F2782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C878CA-B746-4086-82E1-3DD6C6307E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="19392" windowHeight="11520" xr2:uid="{03F52BDC-0433-4116-92CE-69E6036B9E86}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{03F52BDC-0433-4116-92CE-69E6036B9E86}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="568">
   <si>
     <t>#FFFAFA</t>
   </si>
@@ -2122,8 +2122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC391CED-2713-4AA2-A19E-D480A7C8276B}">
   <dimension ref="A1:J292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
-      <selection activeCell="E292" sqref="E292"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="M269" sqref="M269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10229,7 +10229,7 @@
     </row>
     <row r="254" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="B254">
         <v>0</v>
@@ -10246,8 +10246,23 @@
       <c r="F254" t="s">
         <v>523</v>
       </c>
+      <c r="G254">
+        <v>0</v>
+      </c>
+      <c r="H254">
+        <v>0</v>
+      </c>
+      <c r="I254">
+        <v>0</v>
+      </c>
+      <c r="J254">
+        <v>0</v>
+      </c>
     </row>
     <row r="255" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
+        <v>521</v>
+      </c>
       <c r="B255">
         <v>8</v>
       </c>
@@ -10260,8 +10275,26 @@
       <c r="E255" s="1" t="s">
         <v>524</v>
       </c>
+      <c r="F255" t="s">
+        <v>523</v>
+      </c>
+      <c r="G255">
+        <v>0</v>
+      </c>
+      <c r="H255">
+        <v>0</v>
+      </c>
+      <c r="I255">
+        <v>0</v>
+      </c>
+      <c r="J255">
+        <v>0</v>
+      </c>
     </row>
     <row r="256" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A256" t="s">
+        <v>521</v>
+      </c>
       <c r="B256">
         <v>16</v>
       </c>
@@ -10274,8 +10307,26 @@
       <c r="E256" s="1" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="257" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F256" t="s">
+        <v>523</v>
+      </c>
+      <c r="G256">
+        <v>0</v>
+      </c>
+      <c r="H256">
+        <v>0</v>
+      </c>
+      <c r="I256">
+        <v>0</v>
+      </c>
+      <c r="J256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A257" t="s">
+        <v>521</v>
+      </c>
       <c r="B257">
         <v>24</v>
       </c>
@@ -10288,8 +10339,26 @@
       <c r="E257" s="1" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="258" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F257" t="s">
+        <v>523</v>
+      </c>
+      <c r="G257">
+        <v>0</v>
+      </c>
+      <c r="H257">
+        <v>0</v>
+      </c>
+      <c r="I257">
+        <v>0</v>
+      </c>
+      <c r="J257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
+        <v>521</v>
+      </c>
       <c r="B258">
         <v>32</v>
       </c>
@@ -10302,8 +10371,26 @@
       <c r="E258" s="1" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="259" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F258" t="s">
+        <v>523</v>
+      </c>
+      <c r="G258">
+        <v>0</v>
+      </c>
+      <c r="H258">
+        <v>0</v>
+      </c>
+      <c r="I258">
+        <v>0</v>
+      </c>
+      <c r="J258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
+        <v>521</v>
+      </c>
       <c r="B259">
         <v>40</v>
       </c>
@@ -10316,8 +10403,26 @@
       <c r="E259" s="1" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="260" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F259" t="s">
+        <v>523</v>
+      </c>
+      <c r="G259">
+        <v>0</v>
+      </c>
+      <c r="H259">
+        <v>0</v>
+      </c>
+      <c r="I259">
+        <v>0</v>
+      </c>
+      <c r="J259">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A260" t="s">
+        <v>521</v>
+      </c>
       <c r="B260">
         <v>48</v>
       </c>
@@ -10330,8 +10435,26 @@
       <c r="E260" s="1" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="261" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F260" t="s">
+        <v>523</v>
+      </c>
+      <c r="G260">
+        <v>0</v>
+      </c>
+      <c r="H260">
+        <v>0</v>
+      </c>
+      <c r="I260">
+        <v>0</v>
+      </c>
+      <c r="J260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
+        <v>521</v>
+      </c>
       <c r="B261">
         <v>56</v>
       </c>
@@ -10344,8 +10467,26 @@
       <c r="E261" s="1" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="262" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F261" t="s">
+        <v>523</v>
+      </c>
+      <c r="G261">
+        <v>0</v>
+      </c>
+      <c r="H261">
+        <v>0</v>
+      </c>
+      <c r="I261">
+        <v>0</v>
+      </c>
+      <c r="J261">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
+        <v>521</v>
+      </c>
       <c r="B262">
         <v>64</v>
       </c>
@@ -10358,8 +10499,26 @@
       <c r="E262" s="1" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="263" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F262" t="s">
+        <v>523</v>
+      </c>
+      <c r="G262">
+        <v>0</v>
+      </c>
+      <c r="H262">
+        <v>0</v>
+      </c>
+      <c r="I262">
+        <v>0</v>
+      </c>
+      <c r="J262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
+        <v>521</v>
+      </c>
       <c r="B263">
         <v>72</v>
       </c>
@@ -10372,8 +10531,26 @@
       <c r="E263" s="1" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="264" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F263" t="s">
+        <v>523</v>
+      </c>
+      <c r="G263">
+        <v>0</v>
+      </c>
+      <c r="H263">
+        <v>0</v>
+      </c>
+      <c r="I263">
+        <v>0</v>
+      </c>
+      <c r="J263">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
+        <v>521</v>
+      </c>
       <c r="B264">
         <v>80</v>
       </c>
@@ -10386,8 +10563,26 @@
       <c r="E264" s="1" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="265" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F264" t="s">
+        <v>523</v>
+      </c>
+      <c r="G264">
+        <v>0</v>
+      </c>
+      <c r="H264">
+        <v>0</v>
+      </c>
+      <c r="I264">
+        <v>0</v>
+      </c>
+      <c r="J264">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>521</v>
+      </c>
       <c r="B265">
         <v>88</v>
       </c>
@@ -10400,8 +10595,26 @@
       <c r="E265" s="1" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="266" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F265" t="s">
+        <v>523</v>
+      </c>
+      <c r="G265">
+        <v>0</v>
+      </c>
+      <c r="H265">
+        <v>0</v>
+      </c>
+      <c r="I265">
+        <v>0</v>
+      </c>
+      <c r="J265">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
+        <v>521</v>
+      </c>
       <c r="B266">
         <v>96</v>
       </c>
@@ -10414,8 +10627,26 @@
       <c r="E266" s="1" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="267" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F266" t="s">
+        <v>523</v>
+      </c>
+      <c r="G266">
+        <v>0</v>
+      </c>
+      <c r="H266">
+        <v>0</v>
+      </c>
+      <c r="I266">
+        <v>0</v>
+      </c>
+      <c r="J266">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
+        <v>521</v>
+      </c>
       <c r="B267">
         <v>104</v>
       </c>
@@ -10428,8 +10659,26 @@
       <c r="E267" s="1" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="268" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F267" t="s">
+        <v>523</v>
+      </c>
+      <c r="G267">
+        <v>0</v>
+      </c>
+      <c r="H267">
+        <v>0</v>
+      </c>
+      <c r="I267">
+        <v>0</v>
+      </c>
+      <c r="J267">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
+        <v>521</v>
+      </c>
       <c r="B268">
         <v>105</v>
       </c>
@@ -10442,8 +10691,26 @@
       <c r="E268" s="1" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="269" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F268" t="s">
+        <v>523</v>
+      </c>
+      <c r="G268">
+        <v>0</v>
+      </c>
+      <c r="H268">
+        <v>0</v>
+      </c>
+      <c r="I268">
+        <v>0</v>
+      </c>
+      <c r="J268">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
+        <v>521</v>
+      </c>
       <c r="B269">
         <v>112</v>
       </c>
@@ -10456,8 +10723,26 @@
       <c r="E269" s="1" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="270" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F269" t="s">
+        <v>523</v>
+      </c>
+      <c r="G269">
+        <v>0</v>
+      </c>
+      <c r="H269">
+        <v>0</v>
+      </c>
+      <c r="I269">
+        <v>0</v>
+      </c>
+      <c r="J269">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>521</v>
+      </c>
       <c r="B270">
         <v>120</v>
       </c>
@@ -10470,8 +10755,26 @@
       <c r="E270" s="1" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="271" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F270" t="s">
+        <v>523</v>
+      </c>
+      <c r="G270">
+        <v>0</v>
+      </c>
+      <c r="H270">
+        <v>0</v>
+      </c>
+      <c r="I270">
+        <v>0</v>
+      </c>
+      <c r="J270">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A271" t="s">
+        <v>521</v>
+      </c>
       <c r="B271">
         <v>128</v>
       </c>
@@ -10487,8 +10790,23 @@
       <c r="F271" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="272" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G271">
+        <v>0</v>
+      </c>
+      <c r="H271">
+        <v>0</v>
+      </c>
+      <c r="I271">
+        <v>0</v>
+      </c>
+      <c r="J271">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A272" t="s">
+        <v>521</v>
+      </c>
       <c r="B272">
         <v>136</v>
       </c>
@@ -10501,8 +10819,26 @@
       <c r="E272" s="1" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="273" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F272" t="s">
+        <v>521</v>
+      </c>
+      <c r="G272">
+        <v>0</v>
+      </c>
+      <c r="H272">
+        <v>0</v>
+      </c>
+      <c r="I272">
+        <v>0</v>
+      </c>
+      <c r="J272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A273" t="s">
+        <v>521</v>
+      </c>
       <c r="B273">
         <v>144</v>
       </c>
@@ -10515,8 +10851,26 @@
       <c r="E273" s="1" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="274" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F273" t="s">
+        <v>521</v>
+      </c>
+      <c r="G273">
+        <v>0</v>
+      </c>
+      <c r="H273">
+        <v>0</v>
+      </c>
+      <c r="I273">
+        <v>0</v>
+      </c>
+      <c r="J273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
+        <v>521</v>
+      </c>
       <c r="B274">
         <v>152</v>
       </c>
@@ -10529,8 +10883,26 @@
       <c r="E274" s="1" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="275" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F274" t="s">
+        <v>521</v>
+      </c>
+      <c r="G274">
+        <v>0</v>
+      </c>
+      <c r="H274">
+        <v>0</v>
+      </c>
+      <c r="I274">
+        <v>0</v>
+      </c>
+      <c r="J274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A275" t="s">
+        <v>521</v>
+      </c>
       <c r="B275">
         <v>160</v>
       </c>
@@ -10543,8 +10915,26 @@
       <c r="E275" s="1" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="276" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F275" t="s">
+        <v>521</v>
+      </c>
+      <c r="G275">
+        <v>0</v>
+      </c>
+      <c r="H275">
+        <v>0</v>
+      </c>
+      <c r="I275">
+        <v>0</v>
+      </c>
+      <c r="J275">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A276" t="s">
+        <v>521</v>
+      </c>
       <c r="B276">
         <v>168</v>
       </c>
@@ -10557,8 +10947,26 @@
       <c r="E276" s="1" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="277" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F276" t="s">
+        <v>521</v>
+      </c>
+      <c r="G276">
+        <v>0</v>
+      </c>
+      <c r="H276">
+        <v>0</v>
+      </c>
+      <c r="I276">
+        <v>0</v>
+      </c>
+      <c r="J276">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A277" t="s">
+        <v>521</v>
+      </c>
       <c r="B277">
         <v>169</v>
       </c>
@@ -10574,8 +10982,23 @@
       <c r="F277" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="278" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G277">
+        <v>0</v>
+      </c>
+      <c r="H277">
+        <v>0</v>
+      </c>
+      <c r="I277">
+        <v>0</v>
+      </c>
+      <c r="J277">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
+        <v>521</v>
+      </c>
       <c r="B278">
         <v>176</v>
       </c>
@@ -10588,8 +11011,26 @@
       <c r="E278" s="1" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="279" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F278" t="s">
+        <v>546</v>
+      </c>
+      <c r="G278">
+        <v>0</v>
+      </c>
+      <c r="H278">
+        <v>0</v>
+      </c>
+      <c r="I278">
+        <v>0</v>
+      </c>
+      <c r="J278">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
+        <v>521</v>
+      </c>
       <c r="B279">
         <v>184</v>
       </c>
@@ -10602,8 +11043,26 @@
       <c r="E279" s="1" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="280" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F279" t="s">
+        <v>546</v>
+      </c>
+      <c r="G279">
+        <v>0</v>
+      </c>
+      <c r="H279">
+        <v>0</v>
+      </c>
+      <c r="I279">
+        <v>0</v>
+      </c>
+      <c r="J279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A280" t="s">
+        <v>521</v>
+      </c>
       <c r="B280">
         <v>190</v>
       </c>
@@ -10619,8 +11078,23 @@
       <c r="F280" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="281" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G280">
+        <v>0</v>
+      </c>
+      <c r="H280">
+        <v>0</v>
+      </c>
+      <c r="I280">
+        <v>0</v>
+      </c>
+      <c r="J280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A281" t="s">
+        <v>521</v>
+      </c>
       <c r="B281">
         <v>192</v>
       </c>
@@ -10636,8 +11110,23 @@
       <c r="F281" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="282" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G281">
+        <v>0</v>
+      </c>
+      <c r="H281">
+        <v>0</v>
+      </c>
+      <c r="I281">
+        <v>0</v>
+      </c>
+      <c r="J281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
+        <v>521</v>
+      </c>
       <c r="B282">
         <v>200</v>
       </c>
@@ -10650,8 +11139,26 @@
       <c r="E282" s="1" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="283" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F282" t="s">
+        <v>552</v>
+      </c>
+      <c r="G282">
+        <v>0</v>
+      </c>
+      <c r="H282">
+        <v>0</v>
+      </c>
+      <c r="I282">
+        <v>0</v>
+      </c>
+      <c r="J282">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
+        <v>521</v>
+      </c>
       <c r="B283">
         <v>208</v>
       </c>
@@ -10664,8 +11171,26 @@
       <c r="E283" s="1" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="284" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F283" t="s">
+        <v>552</v>
+      </c>
+      <c r="G283">
+        <v>0</v>
+      </c>
+      <c r="H283">
+        <v>0</v>
+      </c>
+      <c r="I283">
+        <v>0</v>
+      </c>
+      <c r="J283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A284" t="s">
+        <v>521</v>
+      </c>
       <c r="B284">
         <v>211</v>
       </c>
@@ -10681,8 +11206,23 @@
       <c r="F284" s="1" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="285" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G284">
+        <v>0</v>
+      </c>
+      <c r="H284">
+        <v>0</v>
+      </c>
+      <c r="I284">
+        <v>0</v>
+      </c>
+      <c r="J284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A285" t="s">
+        <v>521</v>
+      </c>
       <c r="B285">
         <v>216</v>
       </c>
@@ -10695,8 +11235,26 @@
       <c r="E285" s="1" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="286" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F285" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="G285">
+        <v>0</v>
+      </c>
+      <c r="H285">
+        <v>0</v>
+      </c>
+      <c r="I285">
+        <v>0</v>
+      </c>
+      <c r="J285">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
+        <v>521</v>
+      </c>
       <c r="B286">
         <v>220</v>
       </c>
@@ -10712,8 +11270,23 @@
       <c r="F286" s="1" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="287" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G286">
+        <v>0</v>
+      </c>
+      <c r="H286">
+        <v>0</v>
+      </c>
+      <c r="I286">
+        <v>0</v>
+      </c>
+      <c r="J286">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A287" t="s">
+        <v>521</v>
+      </c>
       <c r="B287">
         <v>224</v>
       </c>
@@ -10726,8 +11299,26 @@
       <c r="E287" s="1" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="288" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F287" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="G287">
+        <v>0</v>
+      </c>
+      <c r="H287">
+        <v>0</v>
+      </c>
+      <c r="I287">
+        <v>0</v>
+      </c>
+      <c r="J287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A288" t="s">
+        <v>521</v>
+      </c>
       <c r="B288">
         <v>232</v>
       </c>
@@ -10740,8 +11331,26 @@
       <c r="E288" s="1" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="289" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F288" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="G288">
+        <v>0</v>
+      </c>
+      <c r="H288">
+        <v>0</v>
+      </c>
+      <c r="I288">
+        <v>0</v>
+      </c>
+      <c r="J288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A289" t="s">
+        <v>521</v>
+      </c>
       <c r="B289">
         <v>240</v>
       </c>
@@ -10754,8 +11363,26 @@
       <c r="E289" s="2" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="290" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F289" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="G289">
+        <v>0</v>
+      </c>
+      <c r="H289">
+        <v>0</v>
+      </c>
+      <c r="I289">
+        <v>0</v>
+      </c>
+      <c r="J289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>521</v>
+      </c>
       <c r="B290">
         <v>245</v>
       </c>
@@ -10771,8 +11398,23 @@
       <c r="F290" s="1" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="291" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G290">
+        <v>0</v>
+      </c>
+      <c r="H290">
+        <v>0</v>
+      </c>
+      <c r="I290">
+        <v>0</v>
+      </c>
+      <c r="J290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>521</v>
+      </c>
       <c r="B291">
         <v>248</v>
       </c>
@@ -10785,8 +11427,26 @@
       <c r="E291" s="1" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="292" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F291" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="G291">
+        <v>0</v>
+      </c>
+      <c r="H291">
+        <v>0</v>
+      </c>
+      <c r="I291">
+        <v>0</v>
+      </c>
+      <c r="J291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A292" t="s">
+        <v>566</v>
+      </c>
       <c r="B292">
         <v>255</v>
       </c>
@@ -10801,6 +11461,18 @@
       </c>
       <c r="F292" t="s">
         <v>566</v>
+      </c>
+      <c r="G292">
+        <v>50</v>
+      </c>
+      <c r="H292">
+        <v>50</v>
+      </c>
+      <c r="I292">
+        <v>50</v>
+      </c>
+      <c r="J292">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>